<commit_message>
Create cumulative energy matrix
</commit_message>
<xml_diff>
--- a/SeamCarvingCalculator.xlsx
+++ b/SeamCarvingCalculator.xlsx
@@ -1,22 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duan\OneDrive - The University of Akron\CS435\Projects\P3_SeamCarving\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfgallimore/Code/SeamCarving/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3DBD09-C9DB-DE44-B325-F7246E612896}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="36" windowWidth="16260" windowHeight="6576" tabRatio="270"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" tabRatio="270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -65,7 +75,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,6 +251,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -276,6 +303,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -451,21 +495,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="189" zoomScaleNormal="171" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -479,7 +523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
         <f>B4</f>
         <v>30</v>
@@ -493,7 +537,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>B4</f>
         <v>30</v>
@@ -552,7 +596,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A11" si="3">B5</f>
         <v>215</v>
@@ -611,7 +655,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>45</v>
@@ -670,7 +714,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -729,7 +773,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
         <v>190</v>
@@ -788,7 +832,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -847,7 +891,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -906,7 +950,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f t="shared" si="3"/>
         <v>110</v>
@@ -965,7 +1009,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <f>B11</f>
         <v>110</v>
@@ -979,7 +1023,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -993,7 +1037,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <f>B17</f>
         <v>30</v>
@@ -1016,7 +1060,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f>B17</f>
         <v>30</v>
@@ -1071,7 +1115,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <f t="shared" ref="A18:A24" si="13">B18</f>
         <v>215</v>
@@ -1126,7 +1170,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="13"/>
         <v>135</v>
@@ -1181,7 +1225,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <f t="shared" si="13"/>
         <v>210</v>
@@ -1236,7 +1280,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="13"/>
         <v>41</v>
@@ -1291,7 +1335,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <f t="shared" si="13"/>
         <v>35</v>
@@ -1346,7 +1390,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="13"/>
         <v>5</v>
@@ -1401,7 +1445,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <f t="shared" si="13"/>
         <v>110</v>
@@ -1456,7 +1500,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <f>B24</f>
         <v>110</v>
@@ -1479,7 +1523,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1493,7 +1537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <f>B30</f>
         <v>30</v>
@@ -1516,7 +1560,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <f>B30</f>
         <v>30</v>
@@ -1557,7 +1601,7 @@
         <v>519</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" ref="M30:M36" si="22">I30+MIN(L29:L31)</f>
+        <f t="shared" ref="M30:M33" si="22">I30+MIN(L29:L31)</f>
         <v>611</v>
       </c>
       <c r="N30" s="1"/>
@@ -1571,7 +1615,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" ref="A31:A36" si="23">B31</f>
         <v>215</v>
@@ -1599,7 +1643,7 @@
         <v>307</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" ref="I30:I36" si="26">ABS(D31-E31)+ABS(D31-D30)+ABS(D31-C31)+ABS(D31-D32)</f>
+        <f t="shared" ref="I31:I36" si="26">ABS(D31-E31)+ABS(D31-D30)+ABS(D31-C31)+ABS(D31-D32)</f>
         <v>42</v>
       </c>
       <c r="J31" s="1"/>
@@ -1608,7 +1652,7 @@
         <v>282</v>
       </c>
       <c r="L31" s="2">
-        <f t="shared" ref="L31:L36" si="27">H31+MIN(K30:K32)</f>
+        <f t="shared" ref="L31:L33" si="27">H31+MIN(K30:K32)</f>
         <v>582</v>
       </c>
       <c r="M31" s="4">
@@ -1626,7 +1670,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <f t="shared" si="23"/>
         <v>135</v>
@@ -1681,7 +1725,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="23"/>
         <v>210</v>
@@ -1736,7 +1780,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <f t="shared" si="23"/>
         <v>41</v>
@@ -1773,11 +1817,11 @@
         <v>356</v>
       </c>
       <c r="L34" s="2">
-        <f>H34+MIN(K33:K35)</f>
+        <f t="shared" ref="L34:M36" si="29">H34+MIN(K33:K35)</f>
         <v>672</v>
       </c>
       <c r="M34" s="2">
-        <f>I34+MIN(L33:L35)</f>
+        <f t="shared" si="29"/>
         <v>859</v>
       </c>
       <c r="N34" s="1"/>
@@ -1791,7 +1835,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="23"/>
         <v>5</v>
@@ -1828,11 +1872,11 @@
         <v>236</v>
       </c>
       <c r="L35" s="2">
-        <f>H35+MIN(K34:K36)</f>
+        <f t="shared" si="29"/>
         <v>442</v>
       </c>
       <c r="M35" s="2">
-        <f>I35+MIN(L34:L36)</f>
+        <f t="shared" si="29"/>
         <v>624</v>
       </c>
       <c r="N35" s="1"/>
@@ -1846,7 +1890,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <f t="shared" si="23"/>
         <v>110</v>
@@ -1883,11 +1927,11 @@
         <v>169</v>
       </c>
       <c r="L36" s="2">
-        <f>H36+MIN(K35:K37)</f>
+        <f t="shared" si="29"/>
         <v>444</v>
       </c>
       <c r="M36" s="2">
-        <f>I36+MIN(L35:L37)</f>
+        <f t="shared" si="29"/>
         <v>670</v>
       </c>
       <c r="N36" s="1"/>
@@ -1901,17 +1945,17 @@
         <v>203</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B37" s="1">
         <f>B36</f>
         <v>110</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ref="C37:D37" si="29">C36</f>
+        <f t="shared" ref="C37:D37" si="30">C36</f>
         <v>46</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>203</v>
       </c>
       <c r="K37" s="1">
@@ -1924,7 +1968,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -1938,13 +1982,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B41" s="1">
         <f>B42</f>
         <v>30</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ref="C41" si="30">C42</f>
+        <f t="shared" ref="C41" si="31">C42</f>
         <v>120</v>
       </c>
       <c r="D41" s="1"/>
@@ -1956,7 +2000,7 @@
       </c>
       <c r="M41" s="5"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <f>B42</f>
         <v>30</v>
@@ -1978,13 +2022,13 @@
         <v>275</v>
       </c>
       <c r="H42" s="2">
-        <f t="shared" ref="H42:H49" si="31">ABS(C42-D42)+ABS(C42-C41)+ABS(C42-B42)+ABS(C42-C43)</f>
+        <f t="shared" ref="H42:H49" si="32">ABS(C42-D42)+ABS(C42-C41)+ABS(C42-B42)+ABS(C42-C43)</f>
         <v>168</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="1"/>
       <c r="K42" s="2">
-        <f t="shared" ref="K42:K49" si="32">G42</f>
+        <f t="shared" ref="K42:K49" si="33">G42</f>
         <v>275</v>
       </c>
       <c r="L42" s="2">
@@ -2001,9 +2045,9 @@
       </c>
       <c r="Q42" s="5"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <f t="shared" ref="A43:A49" si="33">B43</f>
+        <f t="shared" ref="A43:A49" si="34">B43</f>
         <v>215</v>
       </c>
       <c r="B43" s="2">
@@ -2013,27 +2057,27 @@
         <v>198</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" ref="D43:D49" si="34">C43</f>
+        <f t="shared" ref="D43:D49" si="35">C43</f>
         <v>198</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="2">
-        <f t="shared" ref="G43:G49" si="35">ABS(B43-C43)+ABS(B43-B42)+ABS(B43-A43)+ABS(B43-B44)</f>
+        <f t="shared" ref="G43:G49" si="36">ABS(B43-C43)+ABS(B43-B42)+ABS(B43-A43)+ABS(B43-B44)</f>
         <v>282</v>
       </c>
       <c r="H43" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>289</v>
       </c>
       <c r="I43" s="5"/>
       <c r="J43" s="1"/>
       <c r="K43" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>282</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" ref="L43:L45" si="36">H43+MIN(K42:K44)</f>
+        <f t="shared" ref="L43:L45" si="37">H43+MIN(K42:K44)</f>
         <v>564</v>
       </c>
       <c r="M43" s="5"/>
@@ -2046,9 +2090,9 @@
       </c>
       <c r="Q43" s="5"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>135</v>
       </c>
       <c r="B44" s="2">
@@ -2058,27 +2102,27 @@
         <v>4</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>4</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>286</v>
       </c>
       <c r="H44" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>573</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="1"/>
       <c r="K44" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>286</v>
       </c>
       <c r="L44" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>708</v>
       </c>
       <c r="M44" s="5"/>
@@ -2091,9 +2135,9 @@
       </c>
       <c r="Q44" s="5"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>210</v>
       </c>
       <c r="B45" s="2">
@@ -2103,27 +2147,27 @@
         <v>252</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>252</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>135</v>
       </c>
       <c r="H45" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>489</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="1"/>
       <c r="K45" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>135</v>
       </c>
       <c r="L45" s="2">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>624</v>
       </c>
       <c r="M45" s="5"/>
@@ -2136,9 +2180,9 @@
       </c>
       <c r="Q45" s="5"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>192</v>
       </c>
       <c r="B46" s="2">
@@ -2148,23 +2192,23 @@
         <v>53</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>53</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>226</v>
       </c>
       <c r="H46" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>409</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="1"/>
       <c r="K46" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>226</v>
       </c>
       <c r="L46" s="2">
@@ -2181,9 +2225,9 @@
       </c>
       <c r="Q46" s="5"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>123</v>
       </c>
       <c r="B47" s="2">
@@ -2193,23 +2237,23 @@
         <v>124</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>124</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>188</v>
       </c>
       <c r="H47" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>80</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="1"/>
       <c r="K47" s="6">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>188</v>
       </c>
       <c r="L47" s="6">
@@ -2226,9 +2270,9 @@
       </c>
       <c r="Q47" s="5"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>5</v>
       </c>
       <c r="B48" s="2">
@@ -2238,27 +2282,27 @@
         <v>132</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>132</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>286</v>
       </c>
       <c r="H48" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>206</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="1"/>
       <c r="K48" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>286</v>
       </c>
       <c r="L48" s="2">
-        <f t="shared" ref="L48:L49" si="37">H48+MIN(K47:K49)</f>
+        <f t="shared" ref="L48:L49" si="38">H48+MIN(K47:K49)</f>
         <v>394</v>
       </c>
       <c r="M48" s="5"/>
@@ -2271,9 +2315,9 @@
       </c>
       <c r="Q48" s="5"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>46</v>
       </c>
       <c r="B49" s="2">
@@ -2283,23 +2327,23 @@
         <v>203</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>203</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>198</v>
       </c>
       <c r="H49" s="2">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>228</v>
       </c>
       <c r="K49" s="2">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>198</v>
       </c>
       <c r="L49" s="2">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>426</v>
       </c>
       <c r="M49" s="5"/>
@@ -2310,7 +2354,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B50" s="1">
         <f>B49</f>
         <v>46</v>
@@ -2326,7 +2370,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>9</v>
       </c>
@@ -2340,13 +2384,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B54" s="1">
         <f>B55</f>
         <v>30</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" ref="C54" si="38">C55</f>
+        <f t="shared" ref="C54" si="39">C55</f>
         <v>120</v>
       </c>
       <c r="D54" s="1"/>
@@ -2358,7 +2402,7 @@
       </c>
       <c r="M54" s="5"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <f>B55</f>
         <v>30</v>
@@ -2380,13 +2424,13 @@
         <v>275</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" ref="H55:H61" si="39">ABS(C55-D55)+ABS(C55-C54)+ABS(C55-B55)+ABS(C55-C56)</f>
+        <f t="shared" ref="H55:H61" si="40">ABS(C55-D55)+ABS(C55-C54)+ABS(C55-B55)+ABS(C55-C56)</f>
         <v>168</v>
       </c>
       <c r="I55" s="5"/>
       <c r="J55" s="1"/>
       <c r="K55" s="2">
-        <f t="shared" ref="K55:K61" si="40">G55</f>
+        <f t="shared" ref="K55:K61" si="41">G55</f>
         <v>275</v>
       </c>
       <c r="L55" s="2">
@@ -2402,9 +2446,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <f t="shared" ref="A56:A61" si="41">B56</f>
+        <f t="shared" ref="A56:A61" si="42">B56</f>
         <v>215</v>
       </c>
       <c r="B56" s="2">
@@ -2414,27 +2458,27 @@
         <v>198</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" ref="D56:D61" si="42">C56</f>
+        <f t="shared" ref="D56:D61" si="43">C56</f>
         <v>198</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="2">
-        <f t="shared" ref="G56:G61" si="43">ABS(B56-C56)+ABS(B56-B55)+ABS(B56-A56)+ABS(B56-B57)</f>
+        <f t="shared" ref="G56:G61" si="44">ABS(B56-C56)+ABS(B56-B55)+ABS(B56-A56)+ABS(B56-B57)</f>
         <v>282</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>289</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="1"/>
       <c r="K56" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>282</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" ref="L56:L58" si="44">H56+MIN(K55:K57)</f>
+        <f t="shared" ref="L56:L58" si="45">H56+MIN(K55:K57)</f>
         <v>564</v>
       </c>
       <c r="M56" s="5"/>
@@ -2446,9 +2490,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>135</v>
       </c>
       <c r="B57" s="2">
@@ -2458,27 +2502,27 @@
         <v>4</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>4</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>286</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>573</v>
       </c>
       <c r="I57" s="5"/>
       <c r="J57" s="1"/>
       <c r="K57" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>286</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>708</v>
       </c>
       <c r="M57" s="5"/>
@@ -2490,9 +2534,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>210</v>
       </c>
       <c r="B58" s="2">
@@ -2502,27 +2546,27 @@
         <v>252</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>252</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>135</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>489</v>
       </c>
       <c r="I58" s="5"/>
       <c r="J58" s="1"/>
       <c r="K58" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>135</v>
       </c>
       <c r="L58" s="2">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>624</v>
       </c>
       <c r="M58" s="5"/>
@@ -2534,9 +2578,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>192</v>
       </c>
       <c r="B59" s="2">
@@ -2546,23 +2590,23 @@
         <v>53</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>53</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="2">
-        <f t="shared" ref="G59:G60" si="45">ABS(B59-C59)+ABS(B59-B58)+ABS(B59-A59)+ABS(B59-B60)</f>
+        <f t="shared" ref="G59:G60" si="46">ABS(B59-C59)+ABS(B59-B58)+ABS(B59-A59)+ABS(B59-B60)</f>
         <v>344</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>417</v>
       </c>
       <c r="I59" s="5"/>
       <c r="J59" s="1"/>
       <c r="K59" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>344</v>
       </c>
       <c r="L59" s="2">
@@ -2578,9 +2622,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>5</v>
       </c>
       <c r="B60" s="2">
@@ -2590,23 +2634,23 @@
         <v>132</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>132</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="2">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>355</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>277</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="1"/>
       <c r="K60" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>355</v>
       </c>
       <c r="L60" s="2">
@@ -2622,9 +2666,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>46</v>
       </c>
       <c r="B61" s="2">
@@ -2634,23 +2678,23 @@
         <v>203</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>203</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>198</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>228</v>
       </c>
       <c r="K61" s="8">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>198</v>
       </c>
       <c r="L61" s="8">
-        <f t="shared" ref="L61" si="46">H61+MIN(K60:K62)</f>
+        <f t="shared" ref="L61" si="47">H61+MIN(K60:K62)</f>
         <v>426</v>
       </c>
       <c r="M61" s="5"/>
@@ -2661,7 +2705,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B62" s="1">
         <f>B61</f>
         <v>46</v>
@@ -2677,7 +2721,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>10</v>
       </c>
@@ -2691,13 +2735,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B66" s="1">
         <f>B67</f>
         <v>30</v>
       </c>
       <c r="C66" s="1">
-        <f t="shared" ref="C66" si="47">C67</f>
+        <f t="shared" ref="C66" si="48">C67</f>
         <v>120</v>
       </c>
       <c r="D66" s="1"/>
@@ -2709,7 +2753,7 @@
       </c>
       <c r="M66" s="5"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <f>B67</f>
         <v>30</v>
@@ -2731,13 +2775,13 @@
         <v>275</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67:H71" si="48">ABS(C67-D67)+ABS(C67-C66)+ABS(C67-B67)+ABS(C67-C68)</f>
+        <f t="shared" ref="H67:H71" si="49">ABS(C67-D67)+ABS(C67-C66)+ABS(C67-B67)+ABS(C67-C68)</f>
         <v>168</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="1"/>
       <c r="K67" s="8">
-        <f t="shared" ref="K67:K72" si="49">G67</f>
+        <f t="shared" ref="K67:K72" si="50">G67</f>
         <v>275</v>
       </c>
       <c r="L67" s="8">
@@ -2753,9 +2797,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <f t="shared" ref="A68:A72" si="50">B68</f>
+        <f t="shared" ref="A68:A72" si="51">B68</f>
         <v>215</v>
       </c>
       <c r="B68" s="2">
@@ -2765,27 +2809,27 @@
         <v>198</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" ref="D68:D72" si="51">C68</f>
+        <f t="shared" ref="D68:D72" si="52">C68</f>
         <v>198</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="2">
-        <f t="shared" ref="G68:H72" si="52">ABS(B68-C68)+ABS(B68-B67)+ABS(B68-A68)+ABS(B68-B69)</f>
+        <f t="shared" ref="G68:H72" si="53">ABS(B68-C68)+ABS(B68-B67)+ABS(B68-A68)+ABS(B68-B69)</f>
         <v>282</v>
       </c>
       <c r="H68" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>289</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="1"/>
       <c r="K68" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>282</v>
       </c>
       <c r="L68" s="2">
-        <f t="shared" ref="L68:L70" si="53">H68+MIN(K67:K69)</f>
+        <f t="shared" ref="L68:L70" si="54">H68+MIN(K67:K69)</f>
         <v>564</v>
       </c>
       <c r="M68" s="5"/>
@@ -2797,9 +2841,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>135</v>
       </c>
       <c r="B69" s="2">
@@ -2809,27 +2853,27 @@
         <v>4</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>4</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>286</v>
       </c>
       <c r="H69" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>573</v>
       </c>
       <c r="I69" s="5"/>
       <c r="J69" s="1"/>
       <c r="K69" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>286</v>
       </c>
       <c r="L69" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>708</v>
       </c>
       <c r="M69" s="5"/>
@@ -2841,9 +2885,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>210</v>
       </c>
       <c r="B70" s="2">
@@ -2853,27 +2897,27 @@
         <v>252</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>252</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>135</v>
       </c>
       <c r="H70" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>489</v>
       </c>
       <c r="I70" s="5"/>
       <c r="J70" s="1"/>
       <c r="K70" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>135</v>
       </c>
       <c r="L70" s="2">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>624</v>
       </c>
       <c r="M70" s="5"/>
@@ -2885,9 +2929,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>192</v>
       </c>
       <c r="B71" s="2">
@@ -2897,23 +2941,23 @@
         <v>53</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>53</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>344</v>
       </c>
       <c r="H71" s="2">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>417</v>
       </c>
       <c r="I71" s="5"/>
       <c r="J71" s="1"/>
       <c r="K71" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>344</v>
       </c>
       <c r="L71" s="2">
@@ -2929,9 +2973,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>5</v>
       </c>
       <c r="B72" s="2">
@@ -2941,23 +2985,23 @@
         <v>132</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>132</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>314</v>
       </c>
       <c r="H72" s="2">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>206</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="1"/>
       <c r="K72" s="2">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>314</v>
       </c>
       <c r="L72" s="2">
@@ -2973,7 +3017,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B73" s="1">
         <f>B72</f>
         <v>5</v>
@@ -2989,7 +3033,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -3003,7 +3047,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B77" s="1">
         <f>B78</f>
         <v>215</v>
@@ -3021,9 +3065,9 @@
       </c>
       <c r="M77" s="5"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <f t="shared" ref="A78:A82" si="54">B78</f>
+        <f t="shared" ref="A78:A82" si="55">B78</f>
         <v>215</v>
       </c>
       <c r="B78" s="2">
@@ -3033,7 +3077,7 @@
         <v>198</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" ref="D78:D82" si="55">C78</f>
+        <f t="shared" ref="D78:D82" si="56">C78</f>
         <v>198</v>
       </c>
       <c r="E78" s="1"/>
@@ -3043,13 +3087,13 @@
         <v>97</v>
       </c>
       <c r="H78" s="2">
-        <f t="shared" ref="H78" si="56">ABS(C78-D78)+ABS(C78-C77)+ABS(C78-B78)+ABS(C78-C79)</f>
+        <f t="shared" ref="H78" si="57">ABS(C78-D78)+ABS(C78-C77)+ABS(C78-B78)+ABS(C78-C79)</f>
         <v>211</v>
       </c>
       <c r="I78" s="5"/>
       <c r="J78" s="1"/>
       <c r="K78" s="8">
-        <f t="shared" ref="K78:K82" si="57">G78</f>
+        <f t="shared" ref="K78:K82" si="58">G78</f>
         <v>97</v>
       </c>
       <c r="L78" s="8">
@@ -3065,9 +3109,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>135</v>
       </c>
       <c r="B79" s="2">
@@ -3077,27 +3121,27 @@
         <v>4</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>4</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="2">
-        <f t="shared" ref="G79:G82" si="58">ABS(B79-C79)+ABS(B79-B78)+ABS(B79-A79)+ABS(B79-B80)</f>
+        <f t="shared" ref="G79:G82" si="59">ABS(B79-C79)+ABS(B79-B78)+ABS(B79-A79)+ABS(B79-B80)</f>
         <v>286</v>
       </c>
       <c r="H79" s="2">
-        <f t="shared" ref="H79:H82" si="59">ABS(C79-D79)+ABS(C79-C78)+ABS(C79-B79)+ABS(C79-C80)</f>
+        <f t="shared" ref="H79:H82" si="60">ABS(C79-D79)+ABS(C79-C78)+ABS(C79-B79)+ABS(C79-C80)</f>
         <v>573</v>
       </c>
       <c r="I79" s="5"/>
       <c r="J79" s="1"/>
       <c r="K79" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>286</v>
       </c>
       <c r="L79" s="2">
-        <f t="shared" ref="L79:L80" si="60">H79+MIN(K78:K80)</f>
+        <f t="shared" ref="L79:L80" si="61">H79+MIN(K78:K80)</f>
         <v>670</v>
       </c>
       <c r="M79" s="5"/>
@@ -3109,9 +3153,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>210</v>
       </c>
       <c r="B80" s="2">
@@ -3121,27 +3165,27 @@
         <v>252</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>252</v>
       </c>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>135</v>
       </c>
       <c r="H80" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>489</v>
       </c>
       <c r="I80" s="5"/>
       <c r="J80" s="1"/>
       <c r="K80" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>135</v>
       </c>
       <c r="L80" s="2">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>624</v>
       </c>
       <c r="M80" s="5"/>
@@ -3153,9 +3197,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>192</v>
       </c>
       <c r="B81" s="2">
@@ -3165,23 +3209,23 @@
         <v>53</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>53</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>344</v>
       </c>
       <c r="H81" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>417</v>
       </c>
       <c r="I81" s="5"/>
       <c r="J81" s="1"/>
       <c r="K81" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>344</v>
       </c>
       <c r="L81" s="2">
@@ -3197,9 +3241,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>5</v>
       </c>
       <c r="B82" s="2">
@@ -3209,23 +3253,23 @@
         <v>132</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>132</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="2">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>314</v>
       </c>
       <c r="H82" s="2">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>206</v>
       </c>
       <c r="I82" s="5"/>
       <c r="J82" s="1"/>
       <c r="K82" s="2">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>314</v>
       </c>
       <c r="L82" s="2">
@@ -3241,7 +3285,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B83" s="1">
         <f>B82</f>
         <v>5</v>
@@ -3257,7 +3301,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>12</v>
       </c>
@@ -3271,7 +3315,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B86" s="1">
         <f>B87</f>
         <v>135</v>
@@ -3289,9 +3333,9 @@
       </c>
       <c r="M86" s="5"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <f t="shared" ref="A87:A90" si="61">B87</f>
+        <f t="shared" ref="A87:A90" si="62">B87</f>
         <v>135</v>
       </c>
       <c r="B87" s="2">
@@ -3301,23 +3345,23 @@
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" ref="D87:D90" si="62">C87</f>
+        <f t="shared" ref="D87:D90" si="63">C87</f>
         <v>4</v>
       </c>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="2">
-        <f t="shared" ref="G87" si="63">ABS(B87-C87)+ABS(B87-B86)+ABS(B87-A87)+ABS(B87-B88)</f>
+        <f t="shared" ref="G87" si="64">ABS(B87-C87)+ABS(B87-B86)+ABS(B87-A87)+ABS(B87-B88)</f>
         <v>206</v>
       </c>
       <c r="H87" s="2">
-        <f t="shared" ref="H87" si="64">ABS(C87-D87)+ABS(C87-C86)+ABS(C87-B87)+ABS(C87-C88)</f>
+        <f t="shared" ref="H87" si="65">ABS(C87-D87)+ABS(C87-C86)+ABS(C87-B87)+ABS(C87-C88)</f>
         <v>379</v>
       </c>
       <c r="I87" s="5"/>
       <c r="J87" s="1"/>
       <c r="K87" s="2">
-        <f t="shared" ref="K87:K90" si="65">G87</f>
+        <f t="shared" ref="K87:K90" si="66">G87</f>
         <v>206</v>
       </c>
       <c r="L87" s="2">
@@ -3333,9 +3377,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>210</v>
       </c>
       <c r="B88" s="2">
@@ -3345,27 +3389,27 @@
         <v>252</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>252</v>
       </c>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="2">
-        <f t="shared" ref="G88:G90" si="66">ABS(B88-C88)+ABS(B88-B87)+ABS(B88-A88)+ABS(B88-B89)</f>
+        <f t="shared" ref="G88:G90" si="67">ABS(B88-C88)+ABS(B88-B87)+ABS(B88-A88)+ABS(B88-B89)</f>
         <v>135</v>
       </c>
       <c r="H88" s="2">
-        <f t="shared" ref="H88:H90" si="67">ABS(C88-D88)+ABS(C88-C87)+ABS(C88-B88)+ABS(C88-C89)</f>
+        <f t="shared" ref="H88:H90" si="68">ABS(C88-D88)+ABS(C88-C87)+ABS(C88-B88)+ABS(C88-C89)</f>
         <v>489</v>
       </c>
       <c r="I88" s="5"/>
       <c r="J88" s="1"/>
       <c r="K88" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>135</v>
       </c>
       <c r="L88" s="2">
-        <f t="shared" ref="L88" si="68">H88+MIN(K87:K89)</f>
+        <f t="shared" ref="L88" si="69">H88+MIN(K87:K89)</f>
         <v>624</v>
       </c>
       <c r="M88" s="5"/>
@@ -3377,9 +3421,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>192</v>
       </c>
       <c r="B89" s="2">
@@ -3389,23 +3433,23 @@
         <v>53</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>53</v>
       </c>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="2">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>344</v>
       </c>
       <c r="H89" s="2">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>417</v>
       </c>
       <c r="I89" s="5"/>
       <c r="J89" s="1"/>
       <c r="K89" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>344</v>
       </c>
       <c r="L89" s="2">
@@ -3421,9 +3465,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <f t="shared" si="61"/>
+        <f t="shared" si="62"/>
         <v>5</v>
       </c>
       <c r="B90" s="2">
@@ -3433,23 +3477,23 @@
         <v>132</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>132</v>
       </c>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="2">
-        <f t="shared" si="66"/>
+        <f t="shared" si="67"/>
         <v>314</v>
       </c>
       <c r="H90" s="2">
-        <f t="shared" si="67"/>
+        <f t="shared" si="68"/>
         <v>206</v>
       </c>
       <c r="I90" s="5"/>
       <c r="J90" s="1"/>
       <c r="K90" s="2">
-        <f t="shared" si="65"/>
+        <f t="shared" si="66"/>
         <v>314</v>
       </c>
       <c r="L90" s="2">
@@ -3465,7 +3509,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B91" s="1">
         <f>B90</f>
         <v>5</v>
@@ -3488,24 +3532,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>